<commit_message>
Revised Input Files and 2D Storage
</commit_message>
<xml_diff>
--- a/CS-180-Joining-an-Organization-Modified.xlsx
+++ b/CS-180-Joining-an-Organization-Modified.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="21405"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\cs180mp2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25600" windowHeight="14620"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="25605" windowHeight="14625"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -252,7 +257,7 @@
     <t>2010-18556</t>
   </si>
   <si>
-    <t>Graduating</t>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -563,7 +568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -573,22 +578,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -640,7 +645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -666,7 +671,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -692,7 +697,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -718,7 +723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -744,7 +749,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -770,7 +775,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -796,7 +801,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -822,7 +827,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -848,7 +853,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -874,7 +879,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -900,7 +905,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -926,7 +931,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -952,7 +957,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -978,7 +983,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -1004,7 +1009,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -1030,7 +1035,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1056,7 +1061,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1082,7 +1087,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -1108,7 +1113,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1134,7 +1139,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1160,7 +1165,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1186,7 +1191,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -1212,7 +1217,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1238,7 +1243,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
@@ -1264,7 +1269,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>50</v>
       </c>
@@ -1290,7 +1295,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>51</v>
       </c>
@@ -1316,7 +1321,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -1342,7 +1347,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1368,7 +1373,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1394,7 +1399,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1420,7 +1425,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>56</v>
       </c>
@@ -1446,7 +1451,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -1472,7 +1477,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -1498,7 +1503,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>60</v>
       </c>
@@ -1524,7 +1529,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -1550,7 +1555,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -1576,7 +1581,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -1602,7 +1607,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>64</v>
       </c>
@@ -1628,7 +1633,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>65</v>
       </c>
@@ -1654,7 +1659,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>66</v>
       </c>
@@ -1680,7 +1685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>67</v>
       </c>
@@ -1706,7 +1711,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>68</v>
       </c>
@@ -1732,7 +1737,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1758,7 +1763,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1784,7 +1789,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -1810,7 +1815,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -1836,7 +1841,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>73</v>
       </c>
@@ -1862,7 +1867,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -1888,7 +1893,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>75</v>
       </c>
@@ -1914,16 +1919,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D55" s="1"/>
     </row>
   </sheetData>

</xml_diff>